<commit_message>
Analyse collected data Collected data is analysed and output as text in the terminal & 3 charts though chart formatting could be improved in the future.
</commit_message>
<xml_diff>
--- a/cornwall_properties.xlsx
+++ b/cornwall_properties.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D52"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,46 +458,46 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>The Laos hut overlooking the Atlantic</t>
+          <t>Cosy Cabin with ...</t>
         </is>
       </c>
       <c r="B2" t="n">
         <v>4.97</v>
       </c>
       <c r="C2" t="n">
-        <v>184</v>
+        <v>92</v>
       </c>
       <c r="D2" t="n">
-        <v>71</v>
+        <v>169</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>The Bothy</t>
+          <t>The Laos hut ove...</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>4.91</v>
+        <v>4.97</v>
       </c>
       <c r="C3" t="n">
-        <v>57</v>
+        <v>184</v>
       </c>
       <c r="D3" t="n">
-        <v>64</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Exceptionally beautiful views!</t>
+          <t>Exceptionally be...</t>
         </is>
       </c>
       <c r="B4" t="n">
         <v>5</v>
       </c>
       <c r="C4" t="n">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D4" t="n">
         <v>88</v>
@@ -506,749 +506,497 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Cosy Cabin with Hot Tub in the Cornish Countryside</t>
+          <t>The Wizards Caul...</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>4.97</v>
+        <v>5</v>
       </c>
       <c r="C5" t="n">
-        <v>90</v>
+        <v>163</v>
       </c>
       <c r="D5" t="n">
-        <v>165</v>
+        <v>176</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Seaweed Suite, Secluded Seaside Stay &amp; Garden View</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr"/>
-      <c r="C6" t="inlineStr"/>
+          <t>Dragonfly Cabin ...</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>4.92</v>
+      </c>
+      <c r="C6" t="n">
+        <v>941</v>
+      </c>
       <c r="D6" t="n">
-        <v>59</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Dragonfly Cabin near Tintagel</t>
+          <t>Little Penlee Gl...</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>4.92</v>
+        <v>5</v>
       </c>
       <c r="C7" t="n">
-        <v>941</v>
+        <v>20</v>
       </c>
       <c r="D7" t="n">
-        <v>76</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Little Dynargh</t>
+          <t>Big blue...</t>
         </is>
       </c>
       <c r="B8" t="n">
         <v>5</v>
       </c>
       <c r="C8" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D8" t="n">
-        <v>73</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Big blue</t>
+          <t>'The Weekender' ...</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>5</v>
+        <v>4.99</v>
       </c>
       <c r="C9" t="n">
-        <v>7</v>
+        <v>512</v>
       </c>
       <c r="D9" t="n">
-        <v>46</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Cosy Cornish Cabin By The Sea</t>
+          <t>Hen’s Roost cabi...</t>
         </is>
       </c>
       <c r="B10" t="n">
         <v>5</v>
       </c>
       <c r="C10" t="n">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="D10" t="n">
-        <v>106</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Delightful shepherd’s hut in peaceful location</t>
+          <t>Romantic Country...</t>
         </is>
       </c>
       <c r="B11" t="n">
         <v>4.96</v>
       </c>
       <c r="C11" t="n">
-        <v>168</v>
+        <v>407</v>
       </c>
       <c r="D11" t="n">
-        <v>87</v>
+        <v>306</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Little Penlee Glamping Pod</t>
+          <t>Luxury Cabin Ret...</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>5</v>
+        <v>4.99</v>
       </c>
       <c r="C12" t="n">
-        <v>20</v>
+        <v>324</v>
       </c>
       <c r="D12" t="n">
-        <v>81</v>
+        <v>203</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>The Wizards Cauldron -Harry Potter Themed</t>
+          <t>Delightful sheph...</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>5</v>
+        <v>4.96</v>
       </c>
       <c r="C13" t="n">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="D13" t="n">
-        <v>176</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Beach House Studio sea view and Coastal path</t>
+          <t>Fistral Retreat...</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>4.87</v>
+        <v>4.96</v>
       </c>
       <c r="C14" t="n">
-        <v>606</v>
+        <v>122</v>
       </c>
       <c r="D14" t="n">
-        <v>100</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Simply paradise.</t>
+          <t>Tranquil Shepher...</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>5</v>
+        <v>4.91</v>
       </c>
       <c r="C15" t="n">
-        <v>33</v>
+        <v>126</v>
       </c>
       <c r="D15" t="n">
-        <v>104</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Studio flat w/ensuite, kitchenette &amp; garden</t>
+          <t>Little Acorn...</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>4.88</v>
+        <v>5</v>
       </c>
       <c r="C16" t="n">
-        <v>548</v>
+        <v>68</v>
       </c>
       <c r="D16" t="n">
-        <v>62</v>
+        <v>163</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Log Cabin</t>
+          <t>Cosy Cornish Cab...</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>4.88</v>
+        <v>5</v>
       </c>
       <c r="C17" t="n">
-        <v>288</v>
+        <v>18</v>
       </c>
       <c r="D17" t="n">
-        <v>54</v>
+        <v>106</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Rosehill Shepherds hut</t>
+          <t>Cozy Ground Floo...</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>5</v>
+        <v>4.91</v>
       </c>
       <c r="C18" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D18" t="n">
-        <v>79</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Surf Cabin, Sauna &amp; Hot Tub</t>
+          <t>Cosy Cabin with ...</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>4.87</v>
+        <v>4.97</v>
       </c>
       <c r="C19" t="n">
-        <v>79</v>
+        <v>92</v>
       </c>
       <c r="D19" t="n">
-        <v>135</v>
+        <v>169</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Cedar Studio with Parking, Central Falmouth</t>
+          <t>The Laos hut ove...</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>4.98</v>
+        <v>4.97</v>
       </c>
       <c r="C20" t="n">
-        <v>611</v>
+        <v>184</v>
       </c>
       <c r="D20" t="n">
-        <v>88</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Travellers Rest</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr"/>
-      <c r="C21" t="inlineStr"/>
+          <t>Exceptionally be...</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>5</v>
+      </c>
+      <c r="C21" t="n">
+        <v>53</v>
+      </c>
       <c r="D21" t="n">
-        <v>127</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Cosy Rural Cabin in the Cornish Countryside</t>
+          <t>The Wizards Caul...</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>4.91</v>
+        <v>5</v>
       </c>
       <c r="C22" t="n">
-        <v>35</v>
+        <v>163</v>
       </c>
       <c r="D22" t="n">
-        <v>120</v>
+        <v>176</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Tiny room by Penzance harbour</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr"/>
-      <c r="C23" t="inlineStr"/>
+          <t>Dragonfly Cabin ...</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>4.92</v>
+      </c>
+      <c r="C23" t="n">
+        <v>941</v>
+      </c>
       <c r="D23" t="n">
-        <v>53</v>
+        <v>76</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Woodmans Hut</t>
+          <t>Little Penlee Gl...</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>4.68</v>
+        <v>5</v>
       </c>
       <c r="C24" t="n">
-        <v>56</v>
+        <v>20</v>
       </c>
       <c r="D24" t="n">
-        <v>93</v>
+        <v>81</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Luxury Cabin Retreat with Hot Tub - Langman</t>
+          <t>Big blue...</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>4.99</v>
+        <v>5</v>
       </c>
       <c r="C25" t="n">
-        <v>322</v>
+        <v>8</v>
       </c>
       <c r="D25" t="n">
-        <v>203</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Buttercup. Vintage feel Caravan. St Eval.</t>
+          <t>Cosy country get...</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>4.88</v>
+        <v>4.9</v>
       </c>
       <c r="C26" t="n">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="D26" t="n">
-        <v>53</v>
+        <v>86</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Little Acorn</t>
+          <t>Aurora Shepherds...</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>5</v>
+        <v>4.97</v>
       </c>
       <c r="C27" t="n">
-        <v>67</v>
+        <v>31</v>
       </c>
       <c r="D27" t="n">
-        <v>162</v>
+        <v>100</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>New! Little Green (Rural stay) Bude</t>
+          <t>Modern &amp; quirky ...</t>
         </is>
       </c>
       <c r="B28" t="n">
         <v>4.96</v>
       </c>
       <c r="C28" t="n">
-        <v>23</v>
+        <v>337</v>
       </c>
       <c r="D28" t="n">
-        <v>98</v>
+        <v>173</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Unique cosy cabin, minutes drive from the sea</t>
+          <t>The Cabin @ The ...</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>4.93</v>
+        <v>4.98</v>
       </c>
       <c r="C29" t="n">
-        <v>234</v>
+        <v>123</v>
       </c>
       <c r="D29" t="n">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Hen’s Roost cabin</t>
+          <t>Spacious room cl...</t>
         </is>
       </c>
       <c r="B30" t="n">
         <v>5</v>
       </c>
       <c r="C30" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D30" t="n">
-        <v>73</v>
+        <v>51</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Ensuite Cabin With A View With A Hot Tub</t>
+          <t>Wildflower Cotta...</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>4.91</v>
+        <v>4.96</v>
       </c>
       <c r="C31" t="n">
-        <v>33</v>
+        <v>147</v>
       </c>
       <c r="D31" t="n">
-        <v>193</v>
+        <v>76</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>The Alt Haus for writers, walkers &amp; solo explorers</t>
+          <t>Chy Vean close t...</t>
         </is>
       </c>
       <c r="B32" t="n">
         <v>5</v>
       </c>
       <c r="C32" t="n">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="D32" t="n">
-        <v>87</v>
+        <v>94</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Wild Willow Camping.</t>
+          <t>Cosy lodge, hot ...</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>4.96</v>
+        <v>5</v>
       </c>
       <c r="C33" t="n">
-        <v>169</v>
+        <v>78</v>
       </c>
       <c r="D33" t="n">
-        <v>75</v>
+        <v>188</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>The Winky Wonky Watershed, a peaceful 1 bed cabin</t>
+          <t>Phoenix Farm She...</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>4.86</v>
+        <v>4.93</v>
       </c>
       <c r="C34" t="n">
-        <v>98</v>
+        <v>458</v>
       </c>
       <c r="D34" t="n">
-        <v>54</v>
+        <v>76</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Hideaway Seaview Pod</t>
+          <t>Relax in Your Pr...</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>4.88</v>
+        <v>4.99</v>
       </c>
       <c r="C35" t="n">
-        <v>48</v>
+        <v>465</v>
       </c>
       <c r="D35" t="n">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>Sweet, rustic cottage for four</t>
-        </is>
-      </c>
-      <c r="B36" t="n">
-        <v>5</v>
-      </c>
-      <c r="C36" t="n">
-        <v>5</v>
-      </c>
-      <c r="D36" t="n">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>Self-catering annexe in a country home</t>
-        </is>
-      </c>
-      <c r="B37" t="n">
-        <v>4.91</v>
-      </c>
-      <c r="C37" t="n">
-        <v>183</v>
-      </c>
-      <c r="D37" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>Convenient &amp; Peaceful Airbnb room</t>
-        </is>
-      </c>
-      <c r="B38" t="n">
-        <v>4.87</v>
-      </c>
-      <c r="C38" t="n">
-        <v>31</v>
-      </c>
-      <c r="D38" t="n">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>Little Maristow</t>
-        </is>
-      </c>
-      <c r="B39" t="n">
-        <v>4.96</v>
-      </c>
-      <c r="C39" t="n">
-        <v>56</v>
-      </c>
-      <c r="D39" t="n">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>Cornish Countryside Escape</t>
-        </is>
-      </c>
-      <c r="B40" t="n">
-        <v>5</v>
-      </c>
-      <c r="C40" t="n">
-        <v>10</v>
-      </c>
-      <c r="D40" t="n">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>Double room with shower room and own entrance</t>
-        </is>
-      </c>
-      <c r="B41" t="n">
-        <v>4.98</v>
-      </c>
-      <c r="C41" t="n">
-        <v>207</v>
-      </c>
-      <c r="D41" t="n">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>Fistral Breeze Apartment</t>
-        </is>
-      </c>
-      <c r="B42" t="inlineStr"/>
-      <c r="C42" t="inlineStr"/>
-      <c r="D42" t="n">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>A fully equipped self-catering holiday apartment.</t>
-        </is>
-      </c>
-      <c r="B43" t="n">
-        <v>4.9</v>
-      </c>
-      <c r="C43" t="n">
-        <v>92</v>
-      </c>
-      <c r="D43" t="n">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>Little Cedar</t>
-        </is>
-      </c>
-      <c r="B44" t="n">
-        <v>5</v>
-      </c>
-      <c r="C44" t="n">
-        <v>3</v>
-      </c>
-      <c r="D44" t="n">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>Martlett Barn</t>
-        </is>
-      </c>
-      <c r="B45" t="n">
-        <v>4.95</v>
-      </c>
-      <c r="C45" t="n">
-        <v>273</v>
-      </c>
-      <c r="D45" t="n">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>Secluded Igluhut and Hot Tub</t>
-        </is>
-      </c>
-      <c r="B46" t="n">
-        <v>4.96</v>
-      </c>
-      <c r="C46" t="n">
-        <v>237</v>
-      </c>
-      <c r="D46" t="n">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>Quiet, luxury en-suite double room with breakfast</t>
-        </is>
-      </c>
-      <c r="B47" t="n">
-        <v>4.99</v>
-      </c>
-      <c r="C47" t="n">
-        <v>244</v>
-      </c>
-      <c r="D47" t="n">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>Lovely sunny double room and private bathroom</t>
-        </is>
-      </c>
-      <c r="B48" t="n">
-        <v>4.86</v>
-      </c>
-      <c r="C48" t="n">
-        <v>238</v>
-      </c>
-      <c r="D48" t="n">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>The Annexe at Pentire</t>
-        </is>
-      </c>
-      <c r="B49" t="n">
-        <v>4.98</v>
-      </c>
-      <c r="C49" t="n">
-        <v>222</v>
-      </c>
-      <c r="D49" t="n">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>Number One: a boutique retreat with free parking.</t>
-        </is>
-      </c>
-      <c r="B50" t="inlineStr"/>
-      <c r="C50" t="inlineStr"/>
-      <c r="D50" t="n">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>Unique self contained chalet with its own garden</t>
-        </is>
-      </c>
-      <c r="B51" t="n">
-        <v>4.79</v>
-      </c>
-      <c r="C51" t="n">
-        <v>414</v>
-      </c>
-      <c r="D51" t="n">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>Basic Single room - No frills.</t>
-        </is>
-      </c>
-      <c r="B52" t="n">
-        <v>4.95</v>
-      </c>
-      <c r="C52" t="n">
-        <v>73</v>
-      </c>
-      <c r="D52" t="n">
-        <v>35</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Stress test program Fixes most issues that arise - may need further stress testing
</commit_message>
<xml_diff>
--- a/cornwall_properties.xlsx
+++ b/cornwall_properties.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -513,7 +513,7 @@
         <v>5</v>
       </c>
       <c r="C5" t="n">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D5" t="n">
         <v>176</v>
@@ -554,17 +554,17 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Big blue...</t>
+          <t>Hen’s Roost cabi...</t>
         </is>
       </c>
       <c r="B8" t="n">
         <v>5</v>
       </c>
       <c r="C8" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D8" t="n">
-        <v>46</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9">
@@ -586,17 +586,17 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Hen’s Roost cabi...</t>
+          <t>Big blue...</t>
         </is>
       </c>
       <c r="B10" t="n">
         <v>5</v>
       </c>
       <c r="C10" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D10" t="n">
-        <v>74</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11">
@@ -618,113 +618,113 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Luxury Cabin Ret...</t>
+          <t>Cosy Cornish Cab...</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>4.99</v>
+        <v>5</v>
       </c>
       <c r="C12" t="n">
-        <v>324</v>
+        <v>18</v>
       </c>
       <c r="D12" t="n">
-        <v>203</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Delightful sheph...</t>
+          <t>Fistral Retreat...</t>
         </is>
       </c>
       <c r="B13" t="n">
         <v>4.96</v>
       </c>
       <c r="C13" t="n">
-        <v>168</v>
+        <v>122</v>
       </c>
       <c r="D13" t="n">
-        <v>87</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Fistral Retreat...</t>
+          <t>Luxury Cabin Ret...</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>4.96</v>
+        <v>4.99</v>
       </c>
       <c r="C14" t="n">
-        <v>122</v>
+        <v>324</v>
       </c>
       <c r="D14" t="n">
-        <v>71</v>
+        <v>203</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Tranquil Shepher...</t>
+          <t>Delightful sheph...</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>4.91</v>
+        <v>4.96</v>
       </c>
       <c r="C15" t="n">
-        <v>126</v>
+        <v>168</v>
       </c>
       <c r="D15" t="n">
-        <v>72</v>
+        <v>87</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Little Acorn...</t>
+          <t>Spacious room cl...</t>
         </is>
       </c>
       <c r="B16" t="n">
         <v>5</v>
       </c>
       <c r="C16" t="n">
-        <v>68</v>
+        <v>3</v>
       </c>
       <c r="D16" t="n">
-        <v>163</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Cosy Cornish Cab...</t>
+          <t>New! Little Gree...</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>5</v>
+        <v>4.96</v>
       </c>
       <c r="C17" t="n">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="D17" t="n">
-        <v>106</v>
+        <v>98</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Cozy Ground Floo...</t>
+          <t>WillowBrook Peac...</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>4.91</v>
+        <v>4.98</v>
       </c>
       <c r="C18" t="n">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D18" t="n">
-        <v>46</v>
+        <v>97</v>
       </c>
     </row>
     <row r="19">
@@ -778,158 +778,158 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>The Wizards Caul...</t>
+          <t>Modern &amp; quirky ...</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>5</v>
+        <v>4.96</v>
       </c>
       <c r="C22" t="n">
-        <v>163</v>
+        <v>337</v>
       </c>
       <c r="D22" t="n">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Dragonfly Cabin ...</t>
+          <t>Little Dynargh...</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>4.92</v>
+        <v>5</v>
       </c>
       <c r="C23" t="n">
-        <v>941</v>
+        <v>6</v>
       </c>
       <c r="D23" t="n">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Little Penlee Gl...</t>
+          <t>Buttercup. Vinta...</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>5</v>
+        <v>4.88</v>
       </c>
       <c r="C24" t="n">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="D24" t="n">
-        <v>81</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Big blue...</t>
+          <t>Glamping at Kead...</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>5</v>
+        <v>4.92</v>
       </c>
       <c r="C25" t="n">
-        <v>8</v>
+        <v>132</v>
       </c>
       <c r="D25" t="n">
-        <v>46</v>
+        <v>81</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Cosy country get...</t>
+          <t>The Bothy...</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>4.9</v>
+        <v>4.91</v>
       </c>
       <c r="C26" t="n">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="D26" t="n">
-        <v>86</v>
+        <v>64</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Aurora Shepherds...</t>
+          <t>Relax in Your Pr...</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>4.97</v>
+        <v>4.99</v>
       </c>
       <c r="C27" t="n">
-        <v>31</v>
+        <v>465</v>
       </c>
       <c r="D27" t="n">
-        <v>100</v>
+        <v>155</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Modern &amp; quirky ...</t>
+          <t>Cosy Rural Cabin...</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>4.96</v>
+        <v>4.92</v>
       </c>
       <c r="C28" t="n">
-        <v>337</v>
+        <v>36</v>
       </c>
       <c r="D28" t="n">
-        <v>173</v>
+        <v>120</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>The Cabin @ The ...</t>
+          <t>Luxury Cabin Ret...</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>4.98</v>
+        <v>5</v>
       </c>
       <c r="C29" t="n">
-        <v>123</v>
+        <v>88</v>
       </c>
       <c r="D29" t="n">
-        <v>77</v>
+        <v>210</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Spacious room cl...</t>
+          <t>Aurora Shepherds...</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>5</v>
+        <v>4.97</v>
       </c>
       <c r="C30" t="n">
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="D30" t="n">
-        <v>51</v>
+        <v>100</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Wildflower Cotta...</t>
+          <t>The Cabin @ The ...</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>4.96</v>
+        <v>4.98</v>
       </c>
       <c r="C31" t="n">
-        <v>147</v>
+        <v>123</v>
       </c>
       <c r="D31" t="n">
         <v>76</v>
@@ -938,65 +938,45 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Chy Vean close t...</t>
+          <t>Off the Beaten S...</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>5</v>
+        <v>4.98</v>
       </c>
       <c r="C32" t="n">
-        <v>54</v>
+        <v>160</v>
       </c>
       <c r="D32" t="n">
-        <v>94</v>
+        <v>108</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Cosy lodge, hot ...</t>
+          <t>Cosy country get...</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>5</v>
+        <v>4.9</v>
       </c>
       <c r="C33" t="n">
-        <v>78</v>
+        <v>50</v>
       </c>
       <c r="D33" t="n">
-        <v>188</v>
+        <v>86</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Phoenix Farm She...</t>
-        </is>
-      </c>
-      <c r="B34" t="n">
-        <v>4.93</v>
-      </c>
-      <c r="C34" t="n">
-        <v>458</v>
-      </c>
+          <t>Seaweed Suite, S...</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr"/>
+      <c r="C34" t="inlineStr"/>
       <c r="D34" t="n">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>Relax in Your Pr...</t>
-        </is>
-      </c>
-      <c r="B35" t="n">
-        <v>4.99</v>
-      </c>
-      <c r="C35" t="n">
-        <v>465</v>
-      </c>
-      <c r="D35" t="n">
-        <v>161</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>